<commit_message>
Built Pyramidal-LSTM encoder-decoder model with attention
</commit_message>
<xml_diff>
--- a/references/reference_summary.xlsx
+++ b/references/reference_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_Statisics\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_Statisics\End2End_Speech_With_Attention\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E7B52-2ED9-452A-9BD2-88D7066AC4F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E093E-3994-4D9F-900A-125AE27377C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B29A0A9-6DBA-4F92-951B-2A7868C90134}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="125">
   <si>
     <t>publish_year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -482,8 +482,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>powered by Google, attention model with pyramid-encoder and decoder structure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEURAL MACHINE TRANSLATION BY JOINTLY LEARNING TO ALIGN AND TRANSLATE</t>
+  </si>
+  <si>
+    <t>Dzmitry Bahdanau, KyungHyun Cho, Yoshua Bengio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bahdanau Attention model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minh-Thang Luong, Hieu Pham, Christopher D. Manning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effective Approaches to Attention-based Neural Machine Translation</t>
   </si>
 </sst>
 </file>
@@ -565,8 +583,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G42" totalsRowShown="0">
-  <autoFilter ref="A1:G42" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G43" totalsRowShown="0">
+  <autoFilter ref="A1:G43" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
     <sortCondition ref="D1:D31"/>
   </sortState>
@@ -880,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213536EA-312D-4C93-A71E-0524F8844C2F}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1638,11 +1656,42 @@
       <c r="E41" t="s">
         <v>109</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="1">
+        <v>43945</v>
+      </c>
+      <c r="G41" t="s">
         <v>119</v>
       </c>
-      <c r="G41" t="s">
-        <v>69</v>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42">
+        <v>2015</v>
+      </c>
+      <c r="C42" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43">
+        <v>2015</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make read wav method into a class named WaveReader
</commit_message>
<xml_diff>
--- a/references/reference_summary.xlsx
+++ b/references/reference_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_Statisics\End2End_Speech_With_Attention\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E093E-3994-4D9F-900A-125AE27377C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FEFC4E-B9D9-455C-A8A6-6F375E2CBCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B29A0A9-6DBA-4F92-951B-2A7868C90134}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
   <si>
     <t>publish_year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -502,6 +502,17 @@
   </si>
   <si>
     <t>Effective Approaches to Attention-based Neural Machine Translation</t>
+  </si>
+  <si>
+    <t>ADAM: A METHOD FOR STOCHASTIC OPTIMIZATION</t>
+  </si>
+  <si>
+    <t>Diederik P. Kingma, Jimmy Lei Ba</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adam optimizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -583,8 +594,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G43" totalsRowShown="0">
-  <autoFilter ref="A1:G43" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G44" totalsRowShown="0">
+  <autoFilter ref="A1:G44" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
     <sortCondition ref="D1:D31"/>
   </sortState>
@@ -898,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213536EA-312D-4C93-A71E-0524F8844C2F}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1694,6 +1705,23 @@
         <v>109</v>
       </c>
     </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44">
+        <v>2015</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish predicting the labels by phonemes
</commit_message>
<xml_diff>
--- a/references/reference_summary.xlsx
+++ b/references/reference_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_Statisics\End2End_Speech_With_Attention\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_Statisics\Speech_With_Encoder_Decoder_Attention\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FEFC4E-B9D9-455C-A8A6-6F375E2CBCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF53B9A-63C4-4968-84FC-8534E1AA806D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B29A0A9-6DBA-4F92-951B-2A7868C90134}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="131">
   <si>
     <t>publish_year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -512,6 +512,17 @@
   </si>
   <si>
     <t>Adam optimizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scene Memory Transformer for Embodied Agents in Long-Horizon Tasks</t>
+  </si>
+  <si>
+    <t>Kuan Fang, Alexander Toshev, Li Fei-Fei, Silvio Savarese</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer powered by Google</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -594,8 +605,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G44" totalsRowShown="0">
-  <autoFilter ref="A1:G44" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G45" totalsRowShown="0">
+  <autoFilter ref="A1:G45" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
     <sortCondition ref="D1:D31"/>
   </sortState>
@@ -909,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213536EA-312D-4C93-A71E-0524F8844C2F}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1602,8 +1613,11 @@
       <c r="E37" t="s">
         <v>109</v>
       </c>
+      <c r="F37" s="1">
+        <v>43970</v>
+      </c>
       <c r="G37" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1720,6 +1734,26 @@
       </c>
       <c r="G44" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45">
+        <v>2019</v>
+      </c>
+      <c r="C45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete Word file for this project
</commit_message>
<xml_diff>
--- a/references/reference_summary.xlsx
+++ b/references/reference_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_Statisics\Speech_With_Encoder_Decoder_Attention\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\北大課程\Project_Statisics\Speech_With_Encoder_Decoder_Attention\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF53B9A-63C4-4968-84FC-8534E1AA806D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B257E214-9221-4841-99BE-4F2D5A0858C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B29A0A9-6DBA-4F92-951B-2A7868C90134}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="139">
   <si>
     <t>publish_year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -523,6 +523,35 @@
   </si>
   <si>
     <t>Transformer powered by Google</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Neural Algorithm of Artistic Style</t>
+  </si>
+  <si>
+    <t>Leon A. Gatys,  Alexander S. Ecker,  Matthias Bethge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>image style change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Going Deeper with Convolutions</t>
+  </si>
+  <si>
+    <t>Christian Szegedy, Wei Liu, Yangqing Jia, Pierre Sermanet, Scott Reed, Dragomir Anguelov, Dumitru Erhan, Vincent Vanhoucke, Andrew Rabinovich</t>
+  </si>
+  <si>
+    <t>image recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inception, average pooling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -605,10 +634,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G45" totalsRowShown="0">
-  <autoFilter ref="A1:G45" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
-    <sortCondition ref="D1:D31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D54B94E-FAC9-4840-AF4F-30F1130E1B0E}" name="表格1" displayName="表格1" ref="A1:G47" totalsRowShown="0">
+  <autoFilter ref="A1:G47" xr:uid="{9BCA467B-90CF-4583-B6B8-020F0A85BC02}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G47">
+    <sortCondition descending="1" ref="B1:B47"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{70A5D719-C622-4045-A300-935B55201F51}" name="paper"/>
@@ -920,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213536EA-312D-4C93-A71E-0524F8844C2F}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -961,459 +990,414 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="B2">
-        <v>1980</v>
+        <v>2019</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>1982</v>
+        <v>2019</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43908</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="B4">
-        <v>1989</v>
+        <v>2019</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="1">
-        <v>43928</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="B5">
-        <v>1994</v>
+        <v>2019</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="1">
-        <v>43924</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B6">
-        <v>1997</v>
+        <v>2018</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="B7">
-        <v>1998</v>
+        <v>2018</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="B8">
-        <v>1999</v>
+        <v>2017</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>109</v>
+      </c>
+      <c r="F8" s="1">
+        <v>43970</v>
+      </c>
+      <c r="G8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="B9">
-        <v>1999</v>
+        <v>2017</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="B10">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B11">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="B12">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B13">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="1">
-        <v>43908</v>
-      </c>
-      <c r="G13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="B14">
-        <v>1975</v>
+        <v>2015</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1">
-        <v>43911</v>
+        <v>133</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="B15">
-        <v>1989</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>2015</v>
+      </c>
+      <c r="C15" t="s">
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="1">
-        <v>43929</v>
+        <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="B16">
-        <v>1995</v>
+        <v>2015</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="1">
-        <v>43907</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="B17">
-        <v>1996</v>
+        <v>2015</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="F17" s="1">
-        <v>43911</v>
+        <v>43945</v>
+      </c>
+      <c r="G17" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="B18">
-        <v>2002</v>
+        <v>2015</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="1">
-        <v>43908</v>
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B19">
-        <v>2004</v>
+        <v>2014</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="B20">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1">
-        <v>43903</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B21">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B22">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="B23">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>137</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B24">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="1">
-        <v>43909</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B25">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="E25" t="s">
         <v>20</v>
@@ -1421,27 +1405,36 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B26">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>85</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G26" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B27">
-        <v>2019</v>
+        <v>2008</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
         <v>23</v>
@@ -1449,146 +1442,161 @@
       <c r="E27" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="1">
-        <v>43908</v>
-      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>1994</v>
+        <v>2008</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F28" s="1">
         <v>43908</v>
       </c>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B29">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="1">
-        <v>43928</v>
-      </c>
-      <c r="G29" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B30">
-        <v>1989</v>
+        <v>2006</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1">
+        <v>43909</v>
+      </c>
+      <c r="G30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="1">
+        <v>43903</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B32">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" t="s">
-        <v>20</v>
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>2016</v>
+        <v>2002</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>29</v>
+      </c>
+      <c r="F33" s="1">
+        <v>43908</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="B34">
-        <v>2019</v>
+        <v>1999</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>18</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>35</v>
       </c>
       <c r="B35">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="B36">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
@@ -1596,164 +1604,225 @@
       <c r="E36" t="s">
         <v>44</v>
       </c>
+      <c r="G36" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="B37">
-        <v>2017</v>
+        <v>1997</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>109</v>
-      </c>
-      <c r="F37" s="1">
-        <v>43970</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>2018</v>
+        <v>1996</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>109</v>
+        <v>38</v>
+      </c>
+      <c r="F38" s="1">
+        <v>43911</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="B39">
-        <v>2017</v>
+        <v>1995</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>109</v>
+        <v>15</v>
+      </c>
+      <c r="F39" s="1">
+        <v>43907</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="B40">
-        <v>2014</v>
+        <v>1994</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>64</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>63</v>
+      </c>
+      <c r="F40" s="1">
+        <v>43924</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="B41">
-        <v>2015</v>
+        <v>1994</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>20</v>
       </c>
       <c r="F41" s="1">
-        <v>43945</v>
-      </c>
-      <c r="G41" t="s">
-        <v>119</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="B42">
-        <v>2015</v>
+        <v>1989</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>109</v>
+        <v>44</v>
+      </c>
+      <c r="F42" s="1">
+        <v>43928</v>
       </c>
       <c r="G42" t="s">
-        <v>122</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="B43">
-        <v>2015</v>
+        <v>1989</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
-      </c>
-      <c r="E43" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>125</v>
+        <v>47</v>
       </c>
       <c r="B44">
-        <v>2015</v>
-      </c>
-      <c r="C44" t="s">
-        <v>126</v>
+        <v>1989</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="1">
+        <v>43929</v>
       </c>
       <c r="G44" t="s">
-        <v>127</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
       <c r="B45">
-        <v>2019</v>
+        <v>1982</v>
       </c>
       <c r="C45" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="G45" t="s">
-        <v>130</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>1980</v>
+      </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47">
+        <v>1975</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="1">
+        <v>43911</v>
+      </c>
+      <c r="G47" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>